<commit_message>
Created excel credentials sheet and sample data sheet
</commit_message>
<xml_diff>
--- a/src/main/java/INOW Automation Data Sheet.xlsx
+++ b/src/main/java/INOW Automation Data Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INOW Testing\src\main\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ADB18A-3730-4F0A-B2A1-AA0281A20161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF8BD53-98AF-430F-A34C-3DA597C0C637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="3" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="8" activeTab="14" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NewBussines" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,9 @@
     <sheet name="Expire" sheetId="20" r:id="rId11"/>
     <sheet name="Place on Hold " sheetId="21" r:id="rId12"/>
     <sheet name="TS_03" sheetId="25" r:id="rId13"/>
-    <sheet name="TS_02" sheetId="35" r:id="rId14"/>
+    <sheet name="Credentials" sheetId="43" r:id="rId14"/>
+    <sheet name="SampleData" sheetId="44" r:id="rId15"/>
+    <sheet name="TS_02" sheetId="35" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4545" uniqueCount="1538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4551" uniqueCount="1544">
   <si>
     <t>NewBussines</t>
   </si>
@@ -4663,6 +4665,24 @@
   </si>
   <si>
     <t xml:space="preserve">reinstatementDescriptions	</t>
+  </si>
+  <si>
+    <t>Credentials</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Not9999!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sample License Number </t>
   </si>
 </sst>
 </file>
@@ -4717,7 +4737,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -4814,11 +4834,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4877,6 +4919,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9062,7 +9115,7 @@
   <dimension ref="A2:AW391"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:AW3"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13031,7 +13084,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13135,10 +13188,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89F98FD-9BB7-400B-BD0D-71C088AB40AD}">
-  <dimension ref="A2:V395"/>
+  <dimension ref="A2:V396"/>
   <sheetViews>
-    <sheetView topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16848,18 +16901,18 @@
       <c r="D369" s="1"/>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A370" s="1"/>
-      <c r="B370" s="7" t="s">
+      <c r="A370" s="26"/>
+      <c r="B370" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C370" s="1" t="s">
+      <c r="C370" s="26" t="s">
         <v>740</v>
       </c>
-      <c r="D370" s="1"/>
+      <c r="D370" s="26"/>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A371" s="1"/>
-      <c r="B371" s="7" t="s">
+      <c r="B371" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C371" s="1" t="s">
@@ -16868,139 +16921,154 @@
       <c r="D371" s="1"/>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A372" s="1"/>
-      <c r="B372" s="7"/>
-      <c r="C372" s="1"/>
-      <c r="D372" s="1"/>
+      <c r="A372" s="25"/>
+      <c r="B372" s="25"/>
+      <c r="C372" s="25"/>
+      <c r="D372" s="25"/>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A373" s="1"/>
-      <c r="B373" s="7"/>
-      <c r="C373" s="1"/>
-      <c r="D373" s="1"/>
+      <c r="A373" s="25"/>
+      <c r="B373" s="25"/>
+      <c r="C373" s="25"/>
+      <c r="D373" s="25"/>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A374" s="1"/>
-      <c r="B374" s="7"/>
-      <c r="C374" s="1"/>
-      <c r="D374" s="1"/>
+      <c r="A374" s="25"/>
+      <c r="B374" s="25"/>
+      <c r="C374" s="25"/>
+      <c r="D374" s="25"/>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A375" s="1"/>
-      <c r="B375" s="7"/>
-      <c r="C375" s="1"/>
-      <c r="D375" s="1"/>
+      <c r="A375" s="25"/>
+      <c r="B375" s="25"/>
+      <c r="C375" s="25"/>
+      <c r="D375" s="25"/>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A376" s="1"/>
-      <c r="B376" s="7"/>
-      <c r="C376" s="1"/>
-      <c r="D376" s="1"/>
+      <c r="A376" s="25"/>
+      <c r="B376" s="25"/>
+      <c r="C376" s="25"/>
+      <c r="D376" s="25"/>
     </row>
     <row r="377" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A377" s="1"/>
-      <c r="B377" s="7"/>
-      <c r="C377" s="1"/>
-      <c r="D377" s="1"/>
+      <c r="A377" s="25"/>
+      <c r="B377" s="25"/>
+      <c r="C377" s="25"/>
+      <c r="D377" s="25"/>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A378" s="1"/>
-      <c r="B378" s="7"/>
-      <c r="C378" s="1"/>
-      <c r="D378" s="1"/>
+      <c r="A378" s="25"/>
+      <c r="B378" s="25"/>
+      <c r="C378" s="25"/>
+      <c r="D378" s="25"/>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A379" s="1"/>
-      <c r="B379" s="7"/>
-      <c r="C379" s="1"/>
-      <c r="D379" s="1"/>
+      <c r="A379" s="25"/>
+      <c r="B379" s="25"/>
+      <c r="C379" s="25"/>
+      <c r="D379" s="25"/>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A380" s="1"/>
-      <c r="B380" s="7"/>
-      <c r="C380" s="1"/>
-      <c r="D380" s="1"/>
+      <c r="A380" s="25"/>
+      <c r="B380" s="25"/>
+      <c r="C380" s="25"/>
+      <c r="D380" s="25"/>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A381" s="1"/>
-      <c r="B381" s="7"/>
-      <c r="C381" s="1"/>
-      <c r="D381" s="1"/>
+      <c r="A381" s="25"/>
+      <c r="B381" s="25"/>
+      <c r="C381" s="25"/>
+      <c r="D381" s="25"/>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A382" s="1"/>
-      <c r="B382" s="7"/>
-      <c r="C382" s="1"/>
-      <c r="D382" s="1"/>
+      <c r="A382" s="25"/>
+      <c r="B382" s="25"/>
+      <c r="C382" s="25"/>
+      <c r="D382" s="25"/>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A383" s="1"/>
-      <c r="B383" s="7"/>
-      <c r="C383" s="1"/>
-      <c r="D383" s="1"/>
+      <c r="A383" s="25"/>
+      <c r="B383" s="25"/>
+      <c r="C383" s="25"/>
+      <c r="D383" s="25"/>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A384" s="1"/>
-      <c r="B384" s="7"/>
-      <c r="C384" s="1"/>
-      <c r="D384" s="1"/>
+      <c r="A384" s="25"/>
+      <c r="B384" s="25"/>
+      <c r="C384" s="25"/>
+      <c r="D384" s="25"/>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A385" s="1"/>
-      <c r="B385" s="7"/>
-      <c r="C385" s="1"/>
-      <c r="D385" s="1"/>
+      <c r="A385" s="25"/>
+      <c r="B385" s="25"/>
+      <c r="C385" s="25"/>
+      <c r="D385" s="25"/>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A386" s="1"/>
-      <c r="B386" s="7"/>
-      <c r="C386" s="1"/>
-      <c r="D386" s="1"/>
+      <c r="A386" s="25"/>
+      <c r="B386" s="25"/>
+      <c r="C386" s="25"/>
+      <c r="D386" s="25"/>
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A387" s="1"/>
-      <c r="B387" s="7"/>
-      <c r="C387" s="1"/>
-      <c r="D387" s="1"/>
+      <c r="A387" s="25"/>
+      <c r="B387" s="25"/>
+      <c r="C387" s="25"/>
+      <c r="D387" s="25"/>
     </row>
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A388" s="1"/>
-      <c r="B388" s="7"/>
-      <c r="C388" s="1"/>
-      <c r="D388" s="1"/>
+      <c r="A388" s="25"/>
+      <c r="B388" s="25"/>
+      <c r="C388" s="25"/>
+      <c r="D388" s="25"/>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A389" s="1"/>
-      <c r="B389" s="7"/>
-      <c r="C389" s="1"/>
-      <c r="D389" s="1"/>
+      <c r="A389" s="25"/>
+      <c r="B389" s="25"/>
+      <c r="C389" s="25"/>
+      <c r="D389" s="25"/>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A390" s="1"/>
-      <c r="B390" s="7"/>
-      <c r="C390" s="1"/>
-      <c r="D390" s="1"/>
+      <c r="A390" s="25"/>
+      <c r="B390" s="25"/>
+      <c r="C390" s="25"/>
+      <c r="D390" s="25"/>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A391" s="1"/>
-      <c r="B391" s="7"/>
-      <c r="C391" s="1"/>
-      <c r="D391" s="1"/>
+      <c r="A391" s="25"/>
+      <c r="B391" s="25"/>
+      <c r="C391" s="25"/>
+      <c r="D391" s="25"/>
     </row>
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A392" s="1"/>
-      <c r="B392" s="7"/>
-      <c r="C392" s="1"/>
-      <c r="D392" s="1"/>
+      <c r="A392" s="25"/>
+      <c r="B392" s="25"/>
+      <c r="C392" s="25"/>
+      <c r="D392" s="25"/>
     </row>
     <row r="393" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A393" s="1"/>
+      <c r="A393" s="25"/>
+      <c r="B393" s="25"/>
+      <c r="C393" s="25"/>
+      <c r="D393" s="25"/>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A394" s="1"/>
+      <c r="A394" s="25"/>
+      <c r="B394" s="25"/>
+      <c r="C394" s="25"/>
+      <c r="D394" s="25"/>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A395" s="1"/>
+      <c r="A395" s="25"/>
+      <c r="B395" s="25"/>
+      <c r="C395" s="25"/>
+      <c r="D395" s="25"/>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A396" s="25"/>
+      <c r="B396" s="25"/>
+      <c r="C396" s="25"/>
+      <c r="D396" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -17018,6 +17086,168 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DA7F691-9AFF-424C-885D-F20749D0C6DC}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="47.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1541</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1540</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1542</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="25"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="30"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BAB4313-CE4A-4214-B5CA-E8D78C1BBB51}">
+  <dimension ref="A2:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B2">
+        <v>11149338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{592B4EC2-F2D6-4387-AB5B-89C605FD6349}">
   <dimension ref="A2:CU395"/>
   <sheetViews>
@@ -28669,8 +28899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7735B18C-A6BE-4010-828D-A7445CCFB55C}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28734,6 +28964,7 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -29008,7 +29239,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29252,7 +29483,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Adding excelclass and Used getter and setter in newbusinessclass
</commit_message>
<xml_diff>
--- a/src/main/java/INOW Automation Data Sheet.xlsx
+++ b/src/main/java/INOW Automation Data Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INOW Testing\src\main\java\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\InsuranceNowAutomation\src\main\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0970F881-E046-485C-9BC1-D9F9E14A6380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29231668-A033-4B5C-B23C-20180BC1A137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="10" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="6" activeTab="11" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NewBussines" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="Rewrite-New " sheetId="18" r:id="rId9"/>
     <sheet name="Expire" sheetId="20" r:id="rId10"/>
     <sheet name="Place on Hold " sheetId="21" r:id="rId11"/>
+    <sheet name="TS_01" sheetId="25" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3056" uniqueCount="1535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3842" uniqueCount="1577">
   <si>
     <t>NewBussines</t>
   </si>
@@ -4651,13 +4652,139 @@
   </si>
   <si>
     <t xml:space="preserve">expireStartTransaction	</t>
+  </si>
+  <si>
+    <t>09/25/2023</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Texas Ranger</t>
+  </si>
+  <si>
+    <t>QATeam</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Jon</t>
+  </si>
+  <si>
+    <t>02/02/1990</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>77478</t>
+  </si>
+  <si>
+    <t>1930 Cheyenne River Cir</t>
+  </si>
+  <si>
+    <t>Sugar Land</t>
+  </si>
+  <si>
+    <t>Email@gmail.com</t>
+  </si>
+  <si>
+    <t>$40,000/$80,000</t>
+  </si>
+  <si>
+    <t>$35,000</t>
+  </si>
+  <si>
+    <t>$1,000</t>
+  </si>
+  <si>
+    <t>Reject</t>
+  </si>
+  <si>
+    <t>newBusinessMedicalPayments</t>
+  </si>
+  <si>
+    <t>newBusinessUninsuredUnderinsuredMotoristBodilyInjury</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Principal</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t>12345687</t>
+  </si>
+  <si>
+    <t>Valid</t>
+  </si>
+  <si>
+    <t>02/02/1980</t>
+  </si>
+  <si>
+    <t>newBusinessDriver1BirthDate</t>
+  </si>
+  <si>
+    <t>04/02/2015</t>
+  </si>
+  <si>
+    <t>newBusinessDriver1DateLicensed</t>
+  </si>
+  <si>
+    <t>Miles</t>
+  </si>
+  <si>
+    <t>Unemployed</t>
+  </si>
+  <si>
+    <t>WAUDGAFL6DA095049</t>
+  </si>
+  <si>
+    <t>To and From Work</t>
+  </si>
+  <si>
+    <t>Owned</t>
+  </si>
+  <si>
+    <t>No Coverage</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>newBusinessVehicle1PurchasedOrLeased</t>
+  </si>
+  <si>
+    <t>newBusinessVehicle1TowingAndLabor</t>
+  </si>
+  <si>
+    <t>newBusinessVehicle1SpecialEquipment</t>
+  </si>
+  <si>
+    <t>newBusinessProducerCode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4680,6 +4807,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4790,10 +4925,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4850,8 +4986,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5166,8 +5306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E708F786-CBCE-421A-AA78-962FE4833BF9}">
   <dimension ref="A2:D395"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A2:D371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5210,7 +5350,9 @@
       <c r="C4" s="5" t="s">
         <v>402</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="24" t="s">
+        <v>1535</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="20"/>
@@ -9131,7 +9273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5456E97C-0A17-42B4-A214-4BA726B8ADBA}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -9231,6 +9373,3831 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA4E5AA-688C-484A-99F1-9AC8F41EC26C}">
+  <dimension ref="A1:D370"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A334" workbookViewId="0">
+      <selection activeCell="C358" sqref="C358"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>401</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>1535</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1537</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1576</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>1538</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="20"/>
+      <c r="B25" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="20"/>
+      <c r="B26" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D26" s="1"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="20"/>
+      <c r="B27" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="20"/>
+      <c r="B28" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
+      <c r="B30" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
+      <c r="B31" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="20"/>
+      <c r="B32" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
+      <c r="B33" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="20"/>
+      <c r="B34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="20"/>
+      <c r="B35" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="20"/>
+      <c r="B36" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="20"/>
+      <c r="B37" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>1547</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="20"/>
+      <c r="B38" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="20"/>
+      <c r="B39" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="20"/>
+      <c r="B40" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="20"/>
+      <c r="B41" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="20"/>
+      <c r="B42" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="20"/>
+      <c r="B43" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="20"/>
+      <c r="B44" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D44" s="26" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="20"/>
+      <c r="B45" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="20"/>
+      <c r="B46" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="20"/>
+      <c r="B47" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="20"/>
+      <c r="B48" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="21"/>
+      <c r="B49" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>1549</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="17"/>
+      <c r="B51" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="D51" s="25" t="s">
+        <v>1550</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="17"/>
+      <c r="B52" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>1553</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="17"/>
+      <c r="B53" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="17"/>
+      <c r="B54" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>1554</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="17"/>
+      <c r="B55" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="17"/>
+      <c r="B56" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="17"/>
+      <c r="B57" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="17"/>
+      <c r="B58" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D58" s="1"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="18"/>
+      <c r="B59" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="17"/>
+      <c r="B61" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="D61" s="1"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="17"/>
+      <c r="B62" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="17"/>
+      <c r="B63" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>1555</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="17"/>
+      <c r="B64" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>1557</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="17"/>
+      <c r="B65" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>1563</v>
+      </c>
+      <c r="D65" s="25" t="s">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="17"/>
+      <c r="B66" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>1558</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="17"/>
+      <c r="B67" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>1559</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="17"/>
+      <c r="B68" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="D68" s="25"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="17"/>
+      <c r="B69" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>1565</v>
+      </c>
+      <c r="D69" s="25" t="s">
+        <v>1564</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="17"/>
+      <c r="B70" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D70" s="1"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="17"/>
+      <c r="B71" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="D71" s="25" t="s">
+        <v>1560</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="17"/>
+      <c r="B72" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>1561</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="17"/>
+      <c r="B73" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="17"/>
+      <c r="B74" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="D74" s="1"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="17"/>
+      <c r="B75" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="D75" s="1"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="17"/>
+      <c r="B76" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="17"/>
+      <c r="B77" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="D77" s="1"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="17"/>
+      <c r="B78" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D78" s="1"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="17"/>
+      <c r="B79" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D79" s="1"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="17"/>
+      <c r="B80" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="D80" s="1"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="17"/>
+      <c r="B81" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="D81" s="1"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="17"/>
+      <c r="B82" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="D82" s="1"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="17"/>
+      <c r="B83" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="D83" s="1"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="17"/>
+      <c r="B84" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="D84" s="1"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="17"/>
+      <c r="B85" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="D85" s="1"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="17"/>
+      <c r="B86" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="D86" s="1"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="17"/>
+      <c r="B87" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D87" s="1"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="17"/>
+      <c r="B88" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="D88" s="1"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="17"/>
+      <c r="B89" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="D89" s="1"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="17"/>
+      <c r="B90" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="D90" s="1"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="17"/>
+      <c r="B91" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="D91" s="1"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="17"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="17"/>
+      <c r="B93" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="D93" s="1"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="17"/>
+      <c r="B94" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="D94" s="1"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="17"/>
+      <c r="B95" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="D95" s="1"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="17"/>
+      <c r="B96" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="D96" s="1"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="17"/>
+      <c r="B97" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="D97" s="1"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="17"/>
+      <c r="B98" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="D98" s="1"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="17"/>
+      <c r="B99" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="D99" s="1"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="17"/>
+      <c r="B100" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="D100" s="1"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="17"/>
+      <c r="B101" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="D101" s="1"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="17"/>
+      <c r="B102" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="D102" s="1"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="17"/>
+      <c r="B103" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="D103" s="1"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="17"/>
+      <c r="B104" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="D104" s="1"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="17"/>
+      <c r="B105" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="D105" s="1"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="17"/>
+      <c r="B106" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="D106" s="1"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="17"/>
+      <c r="B107" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="D107" s="1"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="17"/>
+      <c r="B108" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="D108" s="1"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="17"/>
+      <c r="B109" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D109" s="1"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="17"/>
+      <c r="B110" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="D110" s="1"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="17"/>
+      <c r="B111" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="D111" s="1"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="17"/>
+      <c r="B112" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D112" s="1"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="17"/>
+      <c r="B113" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="D113" s="1"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="17"/>
+      <c r="B114" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="D114" s="1"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="17"/>
+      <c r="B115" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="D115" s="1"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="17"/>
+      <c r="B116" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="D116" s="1"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="17"/>
+      <c r="B117" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="D117" s="1"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="17"/>
+      <c r="B118" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D118" s="1"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="17"/>
+      <c r="B119" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="D119" s="1"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="17"/>
+      <c r="B120" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="D120" s="1"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="17"/>
+      <c r="B121" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="D121" s="1"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="17"/>
+      <c r="B122" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="D122" s="1"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="17"/>
+      <c r="B123" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="D123" s="1"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="17"/>
+      <c r="B124" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="D124" s="1"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="17"/>
+      <c r="B125" s="7"/>
+      <c r="C125" s="1"/>
+      <c r="D125" s="1"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="17"/>
+      <c r="B126" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="D126" s="1"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="17"/>
+      <c r="B127" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="D127" s="1"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="17"/>
+      <c r="B128" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="D128" s="1"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="17"/>
+      <c r="B129" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="D129" s="1"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="17"/>
+      <c r="B130" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="D130" s="1"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="17"/>
+      <c r="B131" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="D131" s="1"/>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="17"/>
+      <c r="B132" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="D132" s="1"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="17"/>
+      <c r="B133" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="D133" s="1"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="17"/>
+      <c r="B134" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="D134" s="1"/>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="17"/>
+      <c r="B135" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="D135" s="1"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="17"/>
+      <c r="B136" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D136" s="1"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="17"/>
+      <c r="B137" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D137" s="1"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="17"/>
+      <c r="B138" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="D138" s="1"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="17"/>
+      <c r="B139" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="D139" s="1"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="17"/>
+      <c r="B140" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="D140" s="1"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="17"/>
+      <c r="B141" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="D141" s="1"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="17"/>
+      <c r="B142" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="D142" s="1"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="17"/>
+      <c r="B143" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C143" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="D143" s="1"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="17"/>
+      <c r="B144" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C144" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="D144" s="1"/>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="17"/>
+      <c r="B145" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C145" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="D145" s="1"/>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="17"/>
+      <c r="B146" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C146" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="D146" s="1"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="17"/>
+      <c r="B147" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C147" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D147" s="1"/>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="17"/>
+      <c r="B148" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C148" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="D148" s="1"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="17"/>
+      <c r="B149" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C149" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="D149" s="1"/>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="17"/>
+      <c r="B150" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="D150" s="1"/>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="17"/>
+      <c r="B151" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="D151" s="1"/>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="17"/>
+      <c r="B152" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C152" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="D152" s="1"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="17"/>
+      <c r="B153" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C153" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="D153" s="1"/>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" s="17"/>
+      <c r="B154" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="D154" s="1"/>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" s="17"/>
+      <c r="B155" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="D155" s="1"/>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" s="17"/>
+      <c r="B156" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D156" s="1"/>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="18"/>
+      <c r="B157" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="D157" s="1"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B158" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D158" s="1"/>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="17"/>
+      <c r="B159" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="D159" s="1"/>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="17"/>
+      <c r="B160" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="D160" s="1"/>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" s="17"/>
+      <c r="B161" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="D161" s="1"/>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" s="17"/>
+      <c r="B162" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>550</v>
+      </c>
+      <c r="D162" s="1"/>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" s="17"/>
+      <c r="B163" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="D163" s="1"/>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" s="17"/>
+      <c r="B164" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="D164" s="1"/>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" s="17"/>
+      <c r="B165" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="D165" s="1"/>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" s="17"/>
+      <c r="B166" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="D166" s="1"/>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" s="17"/>
+      <c r="B167" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="D167" s="1"/>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="17"/>
+      <c r="B168" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="D168" s="1"/>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="17"/>
+      <c r="B169" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="D169" s="1"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="17"/>
+      <c r="B170" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="D170" s="1"/>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" s="17"/>
+      <c r="B171" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="D171" s="1"/>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="17"/>
+      <c r="B172" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="D172" s="1"/>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" s="18"/>
+      <c r="B173" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="D173" s="1"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B174" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="D174" s="25" t="s">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="17"/>
+      <c r="B175" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="D175" s="1"/>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="17"/>
+      <c r="B176" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="D176" s="1"/>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" s="17"/>
+      <c r="B177" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="D177" s="1"/>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="17"/>
+      <c r="B178" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="D178" s="1"/>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" s="17"/>
+      <c r="B179" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D179" s="1"/>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="17"/>
+      <c r="B180" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C180" s="12" t="s">
+        <v>568</v>
+      </c>
+      <c r="D180" s="1"/>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="17"/>
+      <c r="B181" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="D181" s="1"/>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="17"/>
+      <c r="B182" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="D182" s="1"/>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="17"/>
+      <c r="B183" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="D183" s="1"/>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="17"/>
+      <c r="B184" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>1569</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="17"/>
+      <c r="B185" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>1573</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>1570</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="17"/>
+      <c r="B186" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="D186" s="1"/>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="17"/>
+      <c r="B187" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="D187" s="1"/>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" s="17"/>
+      <c r="B188" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="D188" s="1"/>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" s="17"/>
+      <c r="B189" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>577</v>
+      </c>
+      <c r="D189" s="1"/>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" s="17"/>
+      <c r="B190" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="D190" s="1"/>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" s="17"/>
+      <c r="B191" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="17"/>
+      <c r="B192" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" s="17"/>
+      <c r="B193" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="17"/>
+      <c r="B194" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>1574</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="17"/>
+      <c r="B195" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>1575</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="17"/>
+      <c r="B196" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="D196" s="1"/>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="17"/>
+      <c r="B197" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="D197" s="1"/>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="17"/>
+      <c r="B198" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="D198" s="1"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="17"/>
+      <c r="B199" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="D199" s="1"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="17"/>
+      <c r="B200" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>588</v>
+      </c>
+      <c r="D200" s="1"/>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" s="17"/>
+      <c r="B201" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>589</v>
+      </c>
+      <c r="D201" s="1"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="17"/>
+      <c r="B202" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="D202" s="1"/>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="17"/>
+      <c r="B203" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="D203" s="1"/>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="17"/>
+      <c r="B204" s="10"/>
+      <c r="C204" s="1"/>
+      <c r="D204" s="1"/>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="17"/>
+      <c r="B205" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="D205" s="1"/>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="17"/>
+      <c r="B206" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="D206" s="1"/>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="17"/>
+      <c r="B207" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C207" s="1" t="s">
+        <v>594</v>
+      </c>
+      <c r="D207" s="1"/>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="17"/>
+      <c r="B208" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="D208" s="1"/>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A209" s="17"/>
+      <c r="B209" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="D209" s="1"/>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="17"/>
+      <c r="B210" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>597</v>
+      </c>
+      <c r="D210" s="1"/>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="17"/>
+      <c r="B211" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C211" s="12" t="s">
+        <v>598</v>
+      </c>
+      <c r="D211" s="1"/>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="17"/>
+      <c r="B212" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="D212" s="1"/>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="17"/>
+      <c r="B213" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>600</v>
+      </c>
+      <c r="D213" s="1"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="17"/>
+      <c r="B214" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="D214" s="1"/>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" s="17"/>
+      <c r="B215" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="D215" s="1"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="17"/>
+      <c r="B216" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="D216" s="1"/>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="17"/>
+      <c r="B217" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="D217" s="1"/>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="17"/>
+      <c r="B218" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>605</v>
+      </c>
+      <c r="D218" s="1"/>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="17"/>
+      <c r="B219" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C219" s="1" t="s">
+        <v>606</v>
+      </c>
+      <c r="D219" s="1"/>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" s="17"/>
+      <c r="B220" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C220" s="1" t="s">
+        <v>607</v>
+      </c>
+      <c r="D220" s="1"/>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="17"/>
+      <c r="B221" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>608</v>
+      </c>
+      <c r="D221" s="1"/>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="17"/>
+      <c r="B222" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="D222" s="1"/>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" s="17"/>
+      <c r="B223" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>610</v>
+      </c>
+      <c r="D223" s="1"/>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="17"/>
+      <c r="B224" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="D224" s="1"/>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" s="17"/>
+      <c r="B225" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="D225" s="1"/>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="17"/>
+      <c r="B226" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="D226" s="1"/>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="17"/>
+      <c r="B227" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C227" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="D227" s="1"/>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="17"/>
+      <c r="B228" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C228" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="D228" s="1"/>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" s="17"/>
+      <c r="B229" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C229" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="D229" s="1"/>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" s="17"/>
+      <c r="B230" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C230" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="D230" s="1"/>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" s="17"/>
+      <c r="B231" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="D231" s="1"/>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" s="17"/>
+      <c r="B232" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C232" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="D232" s="1"/>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" s="17"/>
+      <c r="B233" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C233" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="D233" s="1"/>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" s="17"/>
+      <c r="B234" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C234" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="D234" s="1"/>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" s="17"/>
+      <c r="B235" s="7"/>
+      <c r="C235" s="1"/>
+      <c r="D235" s="1"/>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" s="17"/>
+      <c r="B236" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C236" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="D236" s="1"/>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" s="17"/>
+      <c r="B237" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C237" s="1" t="s">
+        <v>623</v>
+      </c>
+      <c r="D237" s="1"/>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" s="17"/>
+      <c r="B238" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C238" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="D238" s="1"/>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" s="17"/>
+      <c r="B239" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="D239" s="1"/>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" s="17"/>
+      <c r="B240" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C240" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="D240" s="1"/>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A241" s="17"/>
+      <c r="B241" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C241" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="D241" s="1"/>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="17"/>
+      <c r="B242" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C242" s="12" t="s">
+        <v>628</v>
+      </c>
+      <c r="D242" s="1"/>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" s="17"/>
+      <c r="B243" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="D243" s="1"/>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" s="17"/>
+      <c r="B244" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C244" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="D244" s="1"/>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" s="17"/>
+      <c r="B245" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C245" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="D245" s="1"/>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" s="17"/>
+      <c r="B246" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C246" s="1" t="s">
+        <v>632</v>
+      </c>
+      <c r="D246" s="1"/>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" s="17"/>
+      <c r="B247" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C247" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="D247" s="1"/>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" s="17"/>
+      <c r="B248" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C248" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="D248" s="1"/>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A249" s="17"/>
+      <c r="B249" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C249" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="D249" s="1"/>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" s="17"/>
+      <c r="B250" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C250" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="D250" s="1"/>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" s="17"/>
+      <c r="B251" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="D251" s="1"/>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" s="17"/>
+      <c r="B252" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C252" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="D252" s="1"/>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" s="17"/>
+      <c r="B253" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C253" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="D253" s="1"/>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" s="17"/>
+      <c r="B254" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="D254" s="1"/>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" s="17"/>
+      <c r="B255" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C255" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="D255" s="1"/>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" s="17"/>
+      <c r="B256" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C256" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="D256" s="1"/>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" s="17"/>
+      <c r="B257" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="D257" s="1"/>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" s="17"/>
+      <c r="B258" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C258" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="D258" s="1"/>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" s="17"/>
+      <c r="B259" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C259" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="D259" s="1"/>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" s="17"/>
+      <c r="B260" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="D260" s="1"/>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" s="17"/>
+      <c r="B261" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="D261" s="1"/>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" s="17"/>
+      <c r="B262" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C262" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="D262" s="1"/>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" s="17"/>
+      <c r="B263" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C263" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="D263" s="1"/>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" s="17"/>
+      <c r="B264" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C264" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="D264" s="1"/>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" s="17"/>
+      <c r="B265" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C265" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="D265" s="1"/>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" s="17"/>
+      <c r="B266" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="D266" s="1"/>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" s="17"/>
+      <c r="B267" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C267" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="D267" s="1"/>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" s="17"/>
+      <c r="B268" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="D268" s="1"/>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" s="17"/>
+      <c r="B269" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C269" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="D269" s="1"/>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" s="17"/>
+      <c r="B270" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C270" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D270" s="1"/>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" s="17"/>
+      <c r="B271" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C271" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D271" s="1"/>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" s="17"/>
+      <c r="B272" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C272" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="D272" s="1"/>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" s="17"/>
+      <c r="B273" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C273" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="D273" s="1"/>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" s="17"/>
+      <c r="B274" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C274" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="D274" s="1"/>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" s="17"/>
+      <c r="B275" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="D275" s="1"/>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" s="17"/>
+      <c r="B276" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="D276" s="1"/>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" s="18"/>
+      <c r="B277" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C277" s="12" t="s">
+        <v>762</v>
+      </c>
+      <c r="D277" s="1"/>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B278" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C278" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="D278" s="1"/>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" s="17"/>
+      <c r="B279" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C279" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="D279" s="1"/>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" s="17"/>
+      <c r="B280" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="D280" s="1"/>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A281" s="17"/>
+      <c r="B281" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C281" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="D281" s="1"/>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" s="17"/>
+      <c r="B282" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="D282" s="1"/>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" s="17"/>
+      <c r="B283" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C283" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="D283" s="1"/>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" s="17"/>
+      <c r="B284" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D284" s="1"/>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285" s="17"/>
+      <c r="B285" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="D285" s="1"/>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286" s="17"/>
+      <c r="B286" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C286" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="D286" s="1"/>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" s="17"/>
+      <c r="B287" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="D287" s="1"/>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" s="17"/>
+      <c r="B288" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="D288" s="1"/>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" s="17"/>
+      <c r="B289" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C289" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="D289" s="1"/>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" s="17"/>
+      <c r="B290" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C290" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="D290" s="1"/>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" s="17"/>
+      <c r="B291" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="D291" s="1"/>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" s="17"/>
+      <c r="B292" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="D292" s="1"/>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293" s="17"/>
+      <c r="B293" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C293" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="D293" s="1"/>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294" s="17"/>
+      <c r="B294" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C294" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="D294" s="1"/>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295" s="17"/>
+      <c r="B295" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C295" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="D295" s="1"/>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296" s="17"/>
+      <c r="B296" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="D296" s="1"/>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297" s="17"/>
+      <c r="B297" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="D297" s="1"/>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298" s="17"/>
+      <c r="B298" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C298" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="D298" s="1"/>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299" s="17"/>
+      <c r="B299" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C299" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="D299" s="1"/>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300" s="17"/>
+      <c r="B300" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="D300" s="1"/>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301" s="17"/>
+      <c r="B301" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="D301" s="1"/>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302" s="17"/>
+      <c r="B302" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C302" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="D302" s="1"/>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303" s="17"/>
+      <c r="B303" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="D303" s="1"/>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A304" s="17"/>
+      <c r="B304" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C304" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="D304" s="1"/>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A305" s="17"/>
+      <c r="B305" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="D305" s="1"/>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A306" s="17"/>
+      <c r="B306" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C306" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="D306" s="1"/>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A307" s="17"/>
+      <c r="B307" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="D307" s="1"/>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A308" s="17"/>
+      <c r="B308" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="D308" s="1"/>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A309" s="17"/>
+      <c r="B309" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="D309" s="1"/>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A310" s="17"/>
+      <c r="B310" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="D310" s="1"/>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A311" s="17"/>
+      <c r="B311" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="D311" s="1"/>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A312" s="17"/>
+      <c r="B312" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="D312" s="1"/>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A313" s="17"/>
+      <c r="B313" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C313" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="D313" s="1"/>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A314" s="17"/>
+      <c r="B314" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="D314" s="1"/>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A315" s="17"/>
+      <c r="B315" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="D315" s="1"/>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A316" s="17"/>
+      <c r="B316" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C316" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="D316" s="1"/>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A317" s="17"/>
+      <c r="B317" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="D317" s="1"/>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A318" s="17"/>
+      <c r="B318" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C318" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="D318" s="1"/>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A319" s="17"/>
+      <c r="B319" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="D319" s="1"/>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A320" s="17"/>
+      <c r="B320" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="D320" s="1"/>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A321" s="17"/>
+      <c r="B321" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="D321" s="1"/>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A322" s="17"/>
+      <c r="B322" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C322" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="D322" s="1"/>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A323" s="17"/>
+      <c r="B323" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C323" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="D323" s="1"/>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A324" s="17"/>
+      <c r="B324" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="D324" s="1"/>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A325" s="17"/>
+      <c r="B325" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="D325" s="1"/>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A326" s="17"/>
+      <c r="B326" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C326" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="D326" s="1"/>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A327" s="17"/>
+      <c r="B327" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="D327" s="1"/>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A328" s="17"/>
+      <c r="B328" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="D328" s="1"/>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A329" s="17"/>
+      <c r="B329" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C329" s="12" t="s">
+        <v>700</v>
+      </c>
+      <c r="D329" s="1"/>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A330" s="17"/>
+      <c r="B330" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C330" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="D330" s="1"/>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A331" s="18"/>
+      <c r="B331" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C331" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="D331" s="1"/>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A332" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="B332" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="D332" s="1"/>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A333" s="17"/>
+      <c r="B333" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C333" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="D333" s="1"/>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A334" s="17"/>
+      <c r="B334" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C334" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="D334" s="1"/>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A335" s="17"/>
+      <c r="B335" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>706</v>
+      </c>
+      <c r="D335" s="1"/>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A336" s="17"/>
+      <c r="B336" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="D336" s="1"/>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A337" s="17"/>
+      <c r="B337" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C337" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="D337" s="1"/>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A338" s="17"/>
+      <c r="B338" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C338" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="D338" s="1"/>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A339" s="17"/>
+      <c r="B339" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C339" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="D339" s="1"/>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A340" s="17"/>
+      <c r="B340" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="D340" s="1"/>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A341" s="17"/>
+      <c r="B341" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C341" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="D341" s="1"/>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A342" s="17"/>
+      <c r="B342" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>713</v>
+      </c>
+      <c r="D342" s="1"/>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A343" s="17"/>
+      <c r="B343" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C343" s="1" t="s">
+        <v>714</v>
+      </c>
+      <c r="D343" s="1"/>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A344" s="17"/>
+      <c r="B344" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="D344" s="1"/>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A345" s="17"/>
+      <c r="B345" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="D345" s="1"/>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A346" s="17"/>
+      <c r="B346" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="D346" s="1"/>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A347" s="17"/>
+      <c r="B347" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C347" s="1" t="s">
+        <v>718</v>
+      </c>
+      <c r="D347" s="1"/>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A348" s="17"/>
+      <c r="B348" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C348" s="1" t="s">
+        <v>719</v>
+      </c>
+      <c r="D348" s="1"/>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A349" s="17"/>
+      <c r="B349" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C349" s="1" t="s">
+        <v>720</v>
+      </c>
+      <c r="D349" s="1"/>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A350" s="17"/>
+      <c r="B350" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C350" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="D350" s="1"/>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A351" s="17"/>
+      <c r="B351" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C351" s="1" t="s">
+        <v>722</v>
+      </c>
+      <c r="D351" s="1"/>
+    </row>
+    <row r="352" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A352" s="17"/>
+      <c r="B352" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="D352" s="1"/>
+    </row>
+    <row r="353" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A353" s="18"/>
+      <c r="B353" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C353" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="D353" s="1"/>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A354" s="1"/>
+      <c r="B354" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="D354" s="1"/>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A355" s="1"/>
+      <c r="B355" s="7"/>
+      <c r="C355" s="1" t="s">
+        <v>726</v>
+      </c>
+      <c r="D355" s="1"/>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A356" s="1"/>
+      <c r="B356" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="D356" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A357" s="1"/>
+      <c r="B357" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C357" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="D357" s="1"/>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A358" s="1"/>
+      <c r="B358" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C358" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="D358" s="1" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A359" s="1"/>
+      <c r="B359" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C359" s="1" t="s">
+        <v>730</v>
+      </c>
+      <c r="D359" s="1"/>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A360" s="1"/>
+      <c r="B360" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="D360" s="1"/>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A361" s="1"/>
+      <c r="B361" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C361" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="D361" s="1"/>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A362" s="1"/>
+      <c r="B362" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C362" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="D362" s="1"/>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A363" s="1"/>
+      <c r="B363" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C363" s="1" t="s">
+        <v>734</v>
+      </c>
+      <c r="D363" s="1"/>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A364" s="1"/>
+      <c r="B364" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C364" s="1" t="s">
+        <v>735</v>
+      </c>
+      <c r="D364" s="1"/>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A365" s="1"/>
+      <c r="B365" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C365" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="D365" s="1"/>
+    </row>
+    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A366" s="1"/>
+      <c r="B366" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C366" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="D366" s="1"/>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A367" s="1"/>
+      <c r="B367" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C367" s="1" t="s">
+        <v>738</v>
+      </c>
+      <c r="D367" s="1"/>
+    </row>
+    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A368" s="1"/>
+      <c r="B368" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C368" s="1" t="s">
+        <v>739</v>
+      </c>
+      <c r="D368" s="1"/>
+    </row>
+    <row r="369" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A369" s="1"/>
+      <c r="B369" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C369" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="D369" s="1"/>
+    </row>
+    <row r="370" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A370" s="1"/>
+      <c r="B370" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="D370" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A278:A331"/>
+    <mergeCell ref="A332:A353"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A49"/>
+    <mergeCell ref="A50:A59"/>
+    <mergeCell ref="A60:A157"/>
+    <mergeCell ref="A158:A173"/>
+    <mergeCell ref="A174:A277"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D44" r:id="rId1" xr:uid="{4A029720-88FF-4614-9FFC-D728903A58CE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>